<commit_message>
added the option to itterate the script with different ratios
problem: with small ratio the e-7 imblance problem comes back
</commit_message>
<xml_diff>
--- a/2_bus_input.xlsx
+++ b/2_bus_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304723\Documents\GitHub\CBC_RD_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB2AA94-4F86-45C5-9C54-F9A67B4797FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE3BCFD-5688-4EE3-8CFC-711DE1476B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="6" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="title_page" sheetId="1" r:id="rId1"/>
@@ -537,17 +537,17 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -555,7 +555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -563,7 +563,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -582,9 +582,9 @@
       <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -618,10 +618,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -637,14 +637,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -724,7 +724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -884,27 +884,27 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
@@ -921,17 +921,17 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="3.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
@@ -1184,19 +1184,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D74D64-A296-4AB8-B318-6B84CFC81D10}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1238,10 +1238,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>-10000</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -1268,9 +1268,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>11</v>
@@ -1291,7 +1291,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1314,10 +1314,10 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -1329,24 +1329,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A915C1-4CB9-4DD7-B6E4-10F8FAF3EAA1}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="3"/>
+    <col min="9" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
added CLC function back in script
Last working commit, will now branch to change the CLC function to allow for multiple u[wards and downwards bids per bus
</commit_message>
<xml_diff>
--- a/2_bus_input.xlsx
+++ b/2_bus_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304723\Documents\GitHub\CBC_RD_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE3BCFD-5688-4EE3-8CFC-711DE1476B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D8790B-5A0B-4E6C-974F-4D4E5D072B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="5" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="title_page" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Info &amp; case description</t>
   </si>
@@ -1184,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D74D64-A296-4AB8-B318-6B84CFC81D10}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1206,9 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1240,6 +1242,9 @@
       <c r="C2">
         <v>-150</v>
       </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1250,6 +1255,9 @@
       </c>
       <c r="C3">
         <v>-10000</v>
+      </c>
+      <c r="D3">
+        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1264,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB44F85-5F13-4E40-BB24-6694A7B82B38}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1299,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3">
         <v>23</v>
@@ -1308,10 +1316,10 @@
         <v>18</v>
       </c>
       <c r="F2" s="3">
-        <v>400</v>
+        <v>-400</v>
       </c>
       <c r="G2" s="3">
-        <v>-1000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ensured CHPs are actually limitied if CBC is activated
</commit_message>
<xml_diff>
--- a/2_bus_input.xlsx
+++ b/2_bus_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304723\Documents\GitHub\CBC_RD_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D8790B-5A0B-4E6C-974F-4D4E5D072B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB01E8B8-56C8-4060-9A45-02A14C4FEA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="5" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="title_page" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Info &amp; case description</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>#IMPORTANT: in the RD page include at most one upward and one downward bid per bus</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -1270,15 +1273,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB44F85-5F13-4E40-BB24-6694A7B82B38}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>11</v>
@@ -1298,8 +1301,11 @@
       <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1321,11 +1327,20 @@
       <c r="G2" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more different models
</commit_message>
<xml_diff>
--- a/2_bus_input.xlsx
+++ b/2_bus_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304723\Documents\GitHub\CBC_RD_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB01E8B8-56C8-4060-9A45-02A14C4FEA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCD1975-496B-40F9-9829-A111A7C204A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="title_page" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Info &amp; case description</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>price</t>
-  </si>
-  <si>
-    <t>buy</t>
   </si>
   <si>
     <t>sell</t>
@@ -552,23 +549,23 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +579,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -618,7 +615,7 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -637,7 +634,7 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -735,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -808,84 +805,8 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
-      </c>
-      <c r="I3">
-        <v>100</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-      <c r="K3">
-        <v>100</v>
-      </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="M3">
-        <v>150</v>
-      </c>
-      <c r="N3">
-        <v>150</v>
-      </c>
-      <c r="O3">
-        <v>150</v>
-      </c>
-      <c r="P3">
-        <v>150</v>
-      </c>
-      <c r="Q3">
-        <v>150</v>
-      </c>
-      <c r="R3">
-        <v>150</v>
-      </c>
-      <c r="S3">
-        <v>100</v>
-      </c>
-      <c r="T3">
-        <v>100</v>
-      </c>
-      <c r="U3">
-        <v>100</v>
-      </c>
-      <c r="V3">
-        <v>100</v>
-      </c>
-      <c r="W3">
-        <v>100</v>
-      </c>
-      <c r="X3">
-        <v>100</v>
-      </c>
-      <c r="Y3">
-        <v>100</v>
-      </c>
-      <c r="Z3">
-        <v>100</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -921,14 +842,14 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="26" width="3.5703125" bestFit="1" customWidth="1"/>
@@ -1018,11 +939,11 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
+      <c r="B2" s="1">
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1049,19 +970,19 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>-110</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>-110</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>-110</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1091,86 +1012,6 @@
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
         <v>0</v>
       </c>
     </row>
@@ -1188,7 +1029,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1239,27 +1080,13 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-150</v>
+        <v>-10000</v>
       </c>
       <c r="D2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>-10000</v>
-      </c>
-      <c r="D3">
         <v>600</v>
       </c>
     </row>
@@ -1276,7 +1103,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1302,7 +1129,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1313,19 +1140,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3">
-        <v>-400</v>
+        <v>-100</v>
       </c>
       <c r="G2" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
@@ -1350,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A915C1-4CB9-4DD7-B6E4-10F8FAF3EAA1}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H3" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1369,7 +1196,7 @@
     <col min="9" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1388,54 +1215,17 @@
       <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="H1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="3">
-        <v>400</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>23</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3">
-        <v>-20</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{6e118e09-08be-4360-a815-3fc29828016d}" enabled="1" method="Standard" siteId="{15b734ef-4a07-47e7-90f4-22cc84a7af23}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Models are working, only small changes required
</commit_message>
<xml_diff>
--- a/2_bus_input.xlsx
+++ b/2_bus_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304723\Documents\GitHub\CBC_RD_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCD1975-496B-40F9-9829-A111A7C204A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B529D5C0-6D0D-41EC-A620-72425786338C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="6" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="title_page" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Info &amp; case description</t>
   </si>
@@ -114,13 +114,25 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>conventional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -136,6 +148,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -162,12 +180,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,17 +556,17 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -555,7 +574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -563,7 +582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -579,12 +598,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -601,7 +620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -615,13 +634,13 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -634,17 +653,17 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="6.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -656,402 +675,6 @@
       </c>
       <c r="D1" s="1">
         <v>1</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1">
-        <v>19</v>
-      </c>
-      <c r="W1" s="1">
-        <v>20</v>
-      </c>
-      <c r="X1" s="1">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>150</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD4635E-F3CD-42BC-8B1B-E03EDBB3871B}">
-  <dimension ref="A1:Z4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="3.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1">
-        <v>19</v>
-      </c>
-      <c r="W1" s="1">
-        <v>20</v>
-      </c>
-      <c r="X1" s="1">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>-100</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D74D64-A296-4AB8-B318-6B84CFC81D10}">
-  <dimension ref="A1:Z4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="4.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1076,7 +699,184 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD4635E-F3CD-42BC-8B1B-E03EDBB3871B}">
+  <dimension ref="A1:Z4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="3.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>-40</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D74D64-A296-4AB8-B318-6B84CFC81D10}">
+  <dimension ref="A1:Z4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="4.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1084,13 +884,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-10000</v>
+        <v>-100</v>
       </c>
       <c r="D2">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -1102,14 +902,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB44F85-5F13-4E40-BB24-6694A7B82B38}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1132,12 +934,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -1146,19 +948,19 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3">
-        <v>-100</v>
+        <v>0.1</v>
       </c>
       <c r="G2" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1167,7 +969,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -1177,26 +979,29 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A915C1-4CB9-4DD7-B6E4-10F8FAF3EAA1}">
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="A2:H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="3"/>
+    <col min="9" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1217,6 +1022,58 @@
       </c>
       <c r="H1" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>100</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G3" s="5">
+        <v>100</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>